<commit_message>
Reatraining the quarterly forecast model for PCSunEnergy
</commit_message>
<xml_diff>
--- a/PC SunEnergy/Results_Production_SunEnergy_xgb.xlsx
+++ b/PC SunEnergy/Results_Production_SunEnergy_xgb.xlsx
@@ -28,12 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>20.06.202511</t>
-  </si>
-  <si>
-    <t>20.06.202512</t>
-  </si>
-  <si>
     <t>20.06.202513</t>
   </si>
   <si>
@@ -533,6 +527,12 @@
   </si>
   <si>
     <t>27.06.202511</t>
+  </si>
+  <si>
+    <t>27.06.202512</t>
+  </si>
+  <si>
+    <t>27.06.202513</t>
   </si>
 </sst>
 </file>
@@ -919,7 +919,7 @@
         <v>45828</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0.012</v>
@@ -933,7 +933,7 @@
         <v>45828</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0.012</v>
@@ -947,10 +947,10 @@
         <v>45828</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>2.75</v>
+        <v>3.269</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -961,10 +961,10 @@
         <v>45828</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>2.902</v>
+        <v>2.355</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -975,10 +975,10 @@
         <v>45828</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>2.677</v>
+        <v>1.929</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -989,10 +989,10 @@
         <v>45828</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>2.337</v>
+        <v>1.358</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1003,10 +1003,10 @@
         <v>45828</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>1.929</v>
+        <v>0.613</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1017,10 +1017,10 @@
         <v>45828</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>1.358</v>
+        <v>0.259</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1031,10 +1031,10 @@
         <v>45828</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>0.6</v>
+        <v>0.047</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1045,10 +1045,10 @@
         <v>45828</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>0.259</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1059,10 +1059,10 @@
         <v>45828</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>0.056</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1073,7 +1073,7 @@
         <v>45828</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45828</v>
+        <v>45829</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45828</v>
+        <v>45829</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1115,7 +1115,7 @@
         <v>45829</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>45829</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>45829</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1157,10 +1157,10 @@
         <v>45829</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1171,10 +1171,10 @@
         <v>45829</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.233</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1185,10 +1185,10 @@
         <v>45829</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>0.011</v>
+        <v>0.628</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1199,10 +1199,10 @@
         <v>45829</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>0.233</v>
+        <v>1.552</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1213,10 +1213,10 @@
         <v>45829</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>0.712</v>
+        <v>2.147</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1227,10 +1227,10 @@
         <v>45829</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>1.565</v>
+        <v>2.629</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1241,10 +1241,10 @@
         <v>45829</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>2.217</v>
+        <v>3.223</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1255,10 +1255,10 @@
         <v>45829</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>2.778</v>
+        <v>3.253</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1269,10 +1269,10 @@
         <v>45829</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>3.232</v>
+        <v>3.182</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1283,10 +1283,10 @@
         <v>45829</v>
       </c>
       <c r="B28">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>3.263</v>
+        <v>3.018</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1297,10 +1297,10 @@
         <v>45829</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>3.193</v>
+        <v>2.381</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1311,10 +1311,10 @@
         <v>45829</v>
       </c>
       <c r="B30">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>3.018</v>
+        <v>1.934</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1325,10 +1325,10 @@
         <v>45829</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>2.382</v>
+        <v>1.501</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1339,10 +1339,10 @@
         <v>45829</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>1.949</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1353,10 +1353,10 @@
         <v>45829</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C33">
-        <v>1.46</v>
+        <v>0.303</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1367,10 +1367,10 @@
         <v>45829</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>0.8149999999999999</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1381,10 +1381,10 @@
         <v>45829</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C35">
-        <v>0.303</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1395,10 +1395,10 @@
         <v>45829</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C36">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1409,7 +1409,7 @@
         <v>45829</v>
       </c>
       <c r="B37">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45829</v>
+        <v>45830</v>
       </c>
       <c r="B38">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45829</v>
+        <v>45830</v>
       </c>
       <c r="B39">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>45830</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1465,7 +1465,7 @@
         <v>45830</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>45830</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1493,10 +1493,10 @@
         <v>45830</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1507,10 +1507,10 @@
         <v>45830</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.228</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1521,10 +1521,10 @@
         <v>45830</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>0.018</v>
+        <v>0.701</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1535,10 +1535,10 @@
         <v>45830</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>0.291</v>
+        <v>1.521</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1549,10 +1549,10 @@
         <v>45830</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>0.701</v>
+        <v>2.203</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1563,10 +1563,10 @@
         <v>45830</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>1.521</v>
+        <v>2.81</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1577,10 +1577,10 @@
         <v>45830</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>2.203</v>
+        <v>3.317</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1591,10 +1591,10 @@
         <v>45830</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>2.81</v>
+        <v>3.332</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1605,10 +1605,10 @@
         <v>45830</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>3.317</v>
+        <v>3.351</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1619,10 +1619,10 @@
         <v>45830</v>
       </c>
       <c r="B52">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C52">
-        <v>3.332</v>
+        <v>3.294</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1633,10 +1633,10 @@
         <v>45830</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>3.351</v>
+        <v>2.804</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1647,10 +1647,10 @@
         <v>45830</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>3.294</v>
+        <v>1.983</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1661,10 +1661,10 @@
         <v>45830</v>
       </c>
       <c r="B55">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C55">
-        <v>2.804</v>
+        <v>1.765</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1675,10 +1675,10 @@
         <v>45830</v>
       </c>
       <c r="B56">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>2.044</v>
+        <v>0.92</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1689,10 +1689,10 @@
         <v>45830</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>1.765</v>
+        <v>0.315</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1703,10 +1703,10 @@
         <v>45830</v>
       </c>
       <c r="B58">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>0.9409999999999999</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1717,10 +1717,10 @@
         <v>45830</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C59">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1731,10 +1731,10 @@
         <v>45830</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C60">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1745,7 +1745,7 @@
         <v>45830</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45830</v>
+        <v>45831</v>
       </c>
       <c r="B62">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45830</v>
+        <v>45831</v>
       </c>
       <c r="B63">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>45831</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1801,7 +1801,7 @@
         <v>45831</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>45831</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>45831</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1843,10 +1843,10 @@
         <v>45831</v>
       </c>
       <c r="B68">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.303</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1857,10 +1857,10 @@
         <v>45831</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>0.018</v>
+        <v>0.638</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1871,10 +1871,10 @@
         <v>45831</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>0.303</v>
+        <v>1.508</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1885,10 +1885,10 @@
         <v>45831</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>0.638</v>
+        <v>2.36</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1899,10 +1899,10 @@
         <v>45831</v>
       </c>
       <c r="B72">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>1.508</v>
+        <v>2.867</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1913,10 +1913,10 @@
         <v>45831</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>2.36</v>
+        <v>3.471</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1927,10 +1927,10 @@
         <v>45831</v>
       </c>
       <c r="B74">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C74">
-        <v>2.867</v>
+        <v>3.531</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1941,10 +1941,10 @@
         <v>45831</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>3.471</v>
+        <v>3.392</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1955,10 +1955,10 @@
         <v>45831</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>3.531</v>
+        <v>3.362</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1969,10 +1969,10 @@
         <v>45831</v>
       </c>
       <c r="B77">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C77">
-        <v>3.392</v>
+        <v>2.875</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1983,10 +1983,10 @@
         <v>45831</v>
       </c>
       <c r="B78">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C78">
-        <v>3.362</v>
+        <v>2.137</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1997,10 +1997,10 @@
         <v>45831</v>
       </c>
       <c r="B79">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>2.875</v>
+        <v>1.382</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2011,10 +2011,10 @@
         <v>45831</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C80">
-        <v>2.137</v>
+        <v>0.876</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2025,10 +2025,10 @@
         <v>45831</v>
       </c>
       <c r="B81">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>1.361</v>
+        <v>0.29</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2039,10 +2039,10 @@
         <v>45831</v>
       </c>
       <c r="B82">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C82">
-        <v>0.876</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2053,10 +2053,10 @@
         <v>45831</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C83">
-        <v>0.303</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2067,10 +2067,10 @@
         <v>45831</v>
       </c>
       <c r="B84">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C84">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2081,7 +2081,7 @@
         <v>45831</v>
       </c>
       <c r="B85">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45831</v>
+        <v>45832</v>
       </c>
       <c r="B86">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45831</v>
+        <v>45832</v>
       </c>
       <c r="B87">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2123,7 +2123,7 @@
         <v>45832</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2137,7 +2137,7 @@
         <v>45832</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>45832</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2165,10 +2165,10 @@
         <v>45832</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2179,10 +2179,10 @@
         <v>45832</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.303</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2193,10 +2193,10 @@
         <v>45832</v>
       </c>
       <c r="B93">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C93">
-        <v>0.011</v>
+        <v>0.622</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2207,10 +2207,10 @@
         <v>45832</v>
       </c>
       <c r="B94">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C94">
-        <v>0.236</v>
+        <v>1.556</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2221,10 +2221,10 @@
         <v>45832</v>
       </c>
       <c r="B95">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C95">
-        <v>0.627</v>
+        <v>2.349</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2235,10 +2235,10 @@
         <v>45832</v>
       </c>
       <c r="B96">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C96">
-        <v>1.477</v>
+        <v>2.983</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2249,10 +2249,10 @@
         <v>45832</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C97">
-        <v>2.36</v>
+        <v>3.47</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2263,10 +2263,10 @@
         <v>45832</v>
       </c>
       <c r="B98">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C98">
-        <v>2.858</v>
+        <v>3.533</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2277,10 +2277,10 @@
         <v>45832</v>
       </c>
       <c r="B99">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C99">
-        <v>3.47</v>
+        <v>3.533</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2291,10 +2291,10 @@
         <v>45832</v>
       </c>
       <c r="B100">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C100">
-        <v>3.533</v>
+        <v>3.498</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2305,10 +2305,10 @@
         <v>45832</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C101">
-        <v>3.533</v>
+        <v>3.024</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2319,10 +2319,10 @@
         <v>45832</v>
       </c>
       <c r="B102">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C102">
-        <v>3.498</v>
+        <v>2.246</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2333,10 +2333,10 @@
         <v>45832</v>
       </c>
       <c r="B103">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>3.024</v>
+        <v>1.708</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2347,10 +2347,10 @@
         <v>45832</v>
       </c>
       <c r="B104">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C104">
-        <v>2.246</v>
+        <v>0.913</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2361,10 +2361,10 @@
         <v>45832</v>
       </c>
       <c r="B105">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C105">
-        <v>1.708</v>
+        <v>0.321</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2375,10 +2375,10 @@
         <v>45832</v>
       </c>
       <c r="B106">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>0.913</v>
+        <v>0.099</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2389,10 +2389,10 @@
         <v>45832</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>0.321</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2403,10 +2403,10 @@
         <v>45832</v>
       </c>
       <c r="B108">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C108">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2417,7 +2417,7 @@
         <v>45832</v>
       </c>
       <c r="B109">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="B110">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="B111">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2459,7 +2459,7 @@
         <v>45833</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>45833</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2487,7 +2487,7 @@
         <v>45833</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2501,10 +2501,10 @@
         <v>45833</v>
       </c>
       <c r="B115">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2515,10 +2515,10 @@
         <v>45833</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>0.298</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2529,10 +2529,10 @@
         <v>45833</v>
       </c>
       <c r="B117">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C117">
-        <v>0.011</v>
+        <v>0.629</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2543,10 +2543,10 @@
         <v>45833</v>
       </c>
       <c r="B118">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C118">
-        <v>0.298</v>
+        <v>1.477</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2557,10 +2557,10 @@
         <v>45833</v>
       </c>
       <c r="B119">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C119">
-        <v>0.629</v>
+        <v>2.326</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2571,10 +2571,10 @@
         <v>45833</v>
       </c>
       <c r="B120">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C120">
-        <v>1.477</v>
+        <v>2.855</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2585,10 +2585,10 @@
         <v>45833</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C121">
-        <v>2.326</v>
+        <v>3.432</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2599,10 +2599,10 @@
         <v>45833</v>
       </c>
       <c r="B122">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C122">
-        <v>2.855</v>
+        <v>3.527</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2613,10 +2613,10 @@
         <v>45833</v>
       </c>
       <c r="B123">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C123">
-        <v>3.432</v>
+        <v>3.533</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2627,10 +2627,10 @@
         <v>45833</v>
       </c>
       <c r="B124">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C124">
-        <v>3.527</v>
+        <v>3.362</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2641,10 +2641,10 @@
         <v>45833</v>
       </c>
       <c r="B125">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C125">
-        <v>3.533</v>
+        <v>2.896</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2655,10 +2655,10 @@
         <v>45833</v>
       </c>
       <c r="B126">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C126">
-        <v>3.362</v>
+        <v>1.989</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2669,10 +2669,10 @@
         <v>45833</v>
       </c>
       <c r="B127">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C127">
-        <v>2.896</v>
+        <v>1.296</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2683,10 +2683,10 @@
         <v>45833</v>
       </c>
       <c r="B128">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C128">
-        <v>1.989</v>
+        <v>0.869</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2697,10 +2697,10 @@
         <v>45833</v>
       </c>
       <c r="B129">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C129">
-        <v>1.296</v>
+        <v>0.285</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2711,10 +2711,10 @@
         <v>45833</v>
       </c>
       <c r="B130">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C130">
-        <v>0.869</v>
+        <v>0.063</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2725,10 +2725,10 @@
         <v>45833</v>
       </c>
       <c r="B131">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C131">
-        <v>0.285</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2739,10 +2739,10 @@
         <v>45833</v>
       </c>
       <c r="B132">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C132">
-        <v>0.063</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2753,7 +2753,7 @@
         <v>45833</v>
       </c>
       <c r="B133">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="B134">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="B135">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2795,7 +2795,7 @@
         <v>45834</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2809,7 +2809,7 @@
         <v>45834</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2823,7 +2823,7 @@
         <v>45834</v>
       </c>
       <c r="B138">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2837,10 +2837,10 @@
         <v>45834</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2851,10 +2851,10 @@
         <v>45834</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.298</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2865,10 +2865,10 @@
         <v>45834</v>
       </c>
       <c r="B141">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C141">
-        <v>0.011</v>
+        <v>0.65</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2879,10 +2879,10 @@
         <v>45834</v>
       </c>
       <c r="B142">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C142">
-        <v>0.298</v>
+        <v>1.477</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2893,10 +2893,10 @@
         <v>45834</v>
       </c>
       <c r="B143">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C143">
-        <v>0.65</v>
+        <v>2.352</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2907,10 +2907,10 @@
         <v>45834</v>
       </c>
       <c r="B144">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C144">
-        <v>1.477</v>
+        <v>2.855</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2921,10 +2921,10 @@
         <v>45834</v>
       </c>
       <c r="B145">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C145">
-        <v>2.352</v>
+        <v>3.433</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2935,10 +2935,10 @@
         <v>45834</v>
       </c>
       <c r="B146">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C146">
-        <v>2.855</v>
+        <v>3.53</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2949,10 +2949,10 @@
         <v>45834</v>
       </c>
       <c r="B147">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C147">
-        <v>3.433</v>
+        <v>3.533</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2963,10 +2963,10 @@
         <v>45834</v>
       </c>
       <c r="B148">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C148">
-        <v>3.53</v>
+        <v>3.488</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2977,10 +2977,10 @@
         <v>45834</v>
       </c>
       <c r="B149">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C149">
-        <v>3.533</v>
+        <v>2.981</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2991,10 +2991,10 @@
         <v>45834</v>
       </c>
       <c r="B150">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C150">
-        <v>3.488</v>
+        <v>2.308</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3005,10 +3005,10 @@
         <v>45834</v>
       </c>
       <c r="B151">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C151">
-        <v>2.981</v>
+        <v>1.704</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3019,10 +3019,10 @@
         <v>45834</v>
       </c>
       <c r="B152">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C152">
-        <v>2.308</v>
+        <v>0.901</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3033,10 +3033,10 @@
         <v>45834</v>
       </c>
       <c r="B153">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C153">
-        <v>1.704</v>
+        <v>0.3</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3047,10 +3047,10 @@
         <v>45834</v>
       </c>
       <c r="B154">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>0.901</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3061,10 +3061,10 @@
         <v>45834</v>
       </c>
       <c r="B155">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C155">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3075,10 +3075,10 @@
         <v>45834</v>
       </c>
       <c r="B156">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C156">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3089,7 +3089,7 @@
         <v>45834</v>
       </c>
       <c r="B157">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="B159">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3131,7 +3131,7 @@
         <v>45835</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3145,7 +3145,7 @@
         <v>45835</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3159,7 +3159,7 @@
         <v>45835</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3173,10 +3173,10 @@
         <v>45835</v>
       </c>
       <c r="B163">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3187,10 +3187,10 @@
         <v>45835</v>
       </c>
       <c r="B164">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>0.301</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3201,10 +3201,10 @@
         <v>45835</v>
       </c>
       <c r="B165">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C165">
-        <v>0.011</v>
+        <v>0.64</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3215,10 +3215,10 @@
         <v>45835</v>
       </c>
       <c r="B166">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C166">
-        <v>0.301</v>
+        <v>1.462</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3229,10 +3229,10 @@
         <v>45835</v>
       </c>
       <c r="B167">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C167">
-        <v>0.64</v>
+        <v>2.352</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3243,10 +3243,10 @@
         <v>45835</v>
       </c>
       <c r="B168">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C168">
-        <v>1.462</v>
+        <v>2.858</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3257,10 +3257,10 @@
         <v>45835</v>
       </c>
       <c r="B169">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C169">
-        <v>2.352</v>
+        <v>3.436</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3271,10 +3271,10 @@
         <v>45835</v>
       </c>
       <c r="B170">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C170">
-        <v>2.858</v>
+        <v>3.533</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>